<commit_message>
Script Update for Course -> Skill Weights Master
</commit_message>
<xml_diff>
--- a/02_MasterWifoMannheim/02_Ressources/DB_CourseNames_Notes.xlsx
+++ b/02_MasterWifoMannheim/02_Ressources/DB_CourseNames_Notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailunimannheimde-my.sharepoint.com/personal/pstapf_mail_uni-mannheim_de/Documents/Uni/Master/Masterarbeit/Course_Suggestion/02_MasterWifoMannheim/02_Ressources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="214" documentId="11_AD4DB114E441178AC67DF4B50ED1E6EA693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0FF7D60-AB9F-46D7-B360-67317DAE2B7E}"/>
+  <xr:revisionPtr revIDLastSave="215" documentId="11_AD4DB114E441178AC67DF4B50ED1E6EA693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FD84936-7A1A-4633-8E19-7C2C93C900B9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DB_CourseNames (2)" sheetId="4" r:id="rId1"/>
@@ -1759,12 +1759,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1822,8 +1819,7 @@
   <autoFilter ref="A1:E374" xr:uid="{7D6542BE-F2EF-44B8-99C8-0897D94B7E23}">
     <filterColumn colId="0">
       <filters>
-        <filter val="OPM 504 Transportation II: Air Transport"/>
-        <filter val="OPM 504 Transportation Management: Aviation"/>
+        <filter val="MAN 655  Corporate Strategy: Managing Business Groups"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -2104,7 +2100,7 @@
   <dimension ref="A1:E403"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A322" sqref="A322"/>
+      <selection activeCell="E262" sqref="E262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2228,7 +2224,7 @@
       <c r="D8" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="1" t="s">
         <v>521</v>
       </c>
     </row>
@@ -2385,7 +2381,7 @@
       <c r="D19" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="1" t="s">
         <v>523</v>
       </c>
     </row>
@@ -3312,7 +3308,7 @@
       <c r="D85" t="s">
         <v>10</v>
       </c>
-      <c r="E85" s="2" t="s">
+      <c r="E85" s="1" t="s">
         <v>517</v>
       </c>
     </row>
@@ -3371,7 +3367,7 @@
       <c r="D89" t="s">
         <v>10</v>
       </c>
-      <c r="E89" s="2" t="s">
+      <c r="E89" s="1" t="s">
         <v>518</v>
       </c>
     </row>
@@ -3738,7 +3734,7 @@
       <c r="D115" t="s">
         <v>10</v>
       </c>
-      <c r="E115" s="2" t="s">
+      <c r="E115" s="1" t="s">
         <v>531</v>
       </c>
     </row>
@@ -5113,7 +5109,7 @@
       <c r="D213" t="s">
         <v>10</v>
       </c>
-      <c r="E213" s="2" t="s">
+      <c r="E213" s="1" t="s">
         <v>519</v>
       </c>
     </row>
@@ -5130,7 +5126,7 @@
       <c r="D214" t="s">
         <v>10</v>
       </c>
-      <c r="E214" s="2" t="s">
+      <c r="E214" s="1" t="s">
         <v>543</v>
       </c>
     </row>
@@ -5792,7 +5788,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="262" spans="1:5" hidden="1">
+    <row r="262" spans="1:5">
       <c r="A262" t="s">
         <v>396</v>
       </c>
@@ -5805,7 +5801,7 @@
       <c r="D262" t="s">
         <v>10</v>
       </c>
-      <c r="E262" s="2" t="s">
+      <c r="E262" s="1" t="s">
         <v>544</v>
       </c>
     </row>
@@ -6620,11 +6616,11 @@
       <c r="D320" t="s">
         <v>10</v>
       </c>
-      <c r="E320" s="2" t="s">
+      <c r="E320" s="1" t="s">
         <v>545</v>
       </c>
     </row>
-    <row r="321" spans="1:5">
+    <row r="321" spans="1:5" hidden="1">
       <c r="A321" t="s">
         <v>462</v>
       </c>
@@ -6637,11 +6633,11 @@
       <c r="D321" t="s">
         <v>10</v>
       </c>
-      <c r="E321" s="2" t="s">
+      <c r="E321" s="1" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="322" spans="1:5">
+    <row r="322" spans="1:5" hidden="1">
       <c r="A322" t="s">
         <v>463</v>
       </c>
@@ -6738,7 +6734,7 @@
       <c r="D328" t="s">
         <v>10</v>
       </c>
-      <c r="E328" s="2" t="s">
+      <c r="E328" s="1" t="s">
         <v>547</v>
       </c>
     </row>

</xml_diff>